<commit_message>
update scrumboard sprint 2
</commit_message>
<xml_diff>
--- a/ScrumBoard.xlsx
+++ b/ScrumBoard.xlsx
@@ -23,8 +23,81 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Andy Boets</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">enkel minimum of maximum toevoegen 
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Andy Boets:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+validatie op leeftijd toevoegen</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Andy Boets:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+foto toevoegen van sterrenbeeld op profielpagina</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>backlog</t>
   </si>
@@ -35,15 +108,6 @@
     <t>busy</t>
   </si>
   <si>
-    <t>favorietenlijst</t>
-  </si>
-  <si>
-    <t>html gebruikerspagina 11</t>
-  </si>
-  <si>
-    <t>javascript init gebruikerspagina</t>
-  </si>
-  <si>
     <t>javascript login (6) 4u</t>
   </si>
   <si>
@@ -95,17 +159,35 @@
     <t>Wie</t>
   </si>
   <si>
-    <t>,,,</t>
-  </si>
-  <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>javascript favorietenlijst</t>
+  </si>
+  <si>
+    <t>javascript i feel lucky knop</t>
+  </si>
+  <si>
+    <t>javascript lovecoins, 3 toevoegen , lovecoins verhogen , profielpagina uitbreiden met lovecoins</t>
+  </si>
+  <si>
+    <t>javascript gebruikersprofielpagina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">javascript gebruikersprofielpagina, gegevens wijzigen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">js uitschrijven voor verwijderen van account </t>
+  </si>
+  <si>
+    <t>javascript foto uploaden van mezelf  via webcam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,8 +203,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -132,6 +248,21 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -159,18 +290,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -448,16 +588,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.21875" customWidth="1"/>
+    <col min="1" max="1" width="49.6640625" customWidth="1"/>
     <col min="2" max="2" width="34.21875" customWidth="1"/>
     <col min="3" max="3" width="46.6640625" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
@@ -475,94 +615,100 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="E8" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E8" t="s">
-        <v>11</v>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>